<commit_message>
succesvol 't+3'! Nu een loopje maken voor 't+3'
</commit_message>
<xml_diff>
--- a/predicted_factors_matrix_10.xlsx
+++ b/predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,9 @@
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -448,6 +451,9 @@
       <c r="B2" t="n">
         <v>-5.34045850919005</v>
       </c>
+      <c r="C2" t="n">
+        <v>-5.041423880421429</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -456,6 +462,9 @@
       <c r="B3" t="n">
         <v>-1.131202972523497</v>
       </c>
+      <c r="C3" t="n">
+        <v>-1.155700669620174</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -464,6 +473,9 @@
       <c r="B4" t="n">
         <v>-0.1981644286802984</v>
       </c>
+      <c r="C4" t="n">
+        <v>-0.07506705564893197</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -472,6 +484,9 @@
       <c r="B5" t="n">
         <v>-0.7595660621586662</v>
       </c>
+      <c r="C5" t="n">
+        <v>-0.4238602485323116</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -480,6 +495,9 @@
       <c r="B6" t="n">
         <v>0.07734033066112114</v>
       </c>
+      <c r="C6" t="n">
+        <v>0.01520034001876744</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -488,6 +506,9 @@
       <c r="B7" t="n">
         <v>0.1439439259330764</v>
       </c>
+      <c r="C7" t="n">
+        <v>0.1043279679824023</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -496,6 +517,9 @@
       <c r="B8" t="n">
         <v>0.2380344147737066</v>
       </c>
+      <c r="C8" t="n">
+        <v>0.1352696695087812</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -504,6 +528,9 @@
       <c r="B9" t="n">
         <v>0.03166756318959256</v>
       </c>
+      <c r="C9" t="n">
+        <v>0.02787891322180851</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -512,6 +539,9 @@
       <c r="B10" t="n">
         <v>0.03053534835443629</v>
       </c>
+      <c r="C10" t="n">
+        <v>0.02331057633078736</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -519,6 +549,9 @@
       </c>
       <c r="B11" t="n">
         <v>0.003002641750018904</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.006819328375059187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loopje runt, maar geef andere getallen dan voor de loop.
</commit_message>
<xml_diff>
--- a/predicted_factors_matrix_10.xlsx
+++ b/predicted_factors_matrix_10.xlsx
@@ -452,7 +452,7 @@
         <v>-5.34045850919005</v>
       </c>
       <c r="C2" t="n">
-        <v>-5.041423880421429</v>
+        <v>-5.023377998469892</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         <v>-1.131202972523497</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.155700669620174</v>
+        <v>-1.151483576865103</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         <v>-0.1981644286802984</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.07506705564893197</v>
+        <v>-0.06510371792358649</v>
       </c>
     </row>
     <row r="5">
@@ -485,7 +485,7 @@
         <v>-0.7595660621586662</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4238602485323116</v>
+        <v>-0.4130396773035255</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         <v>0.07734033066112114</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01520034001876744</v>
+        <v>0.01420778898168975</v>
       </c>
     </row>
     <row r="7">
@@ -507,7 +507,7 @@
         <v>0.1439439259330764</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1043279679824023</v>
+        <v>0.1031345171695419</v>
       </c>
     </row>
     <row r="8">
@@ -518,7 +518,7 @@
         <v>0.2380344147737066</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1352696695087812</v>
+        <v>0.1337589614876022</v>
       </c>
     </row>
     <row r="9">
@@ -529,7 +529,7 @@
         <v>0.03166756318959256</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02787891322180851</v>
+        <v>0.02733475124857185</v>
       </c>
     </row>
     <row r="10">
@@ -540,7 +540,7 @@
         <v>0.03053534835443629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02331057633078736</v>
+        <v>0.0234479315146108</v>
       </c>
     </row>
     <row r="11">
@@ -551,7 +551,7 @@
         <v>0.003002641750018904</v>
       </c>
       <c r="C11" t="n">
-        <v>0.006819328375059187</v>
+        <v>0.006722294386397641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
't+5' nu gelukt handmatig, probeer nu kolom namen aan te passen
</commit_message>
<xml_diff>
--- a/predicted_factors_matrix_10.xlsx
+++ b/predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,12 @@
       <c r="C1" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,7 +458,13 @@
         <v>-5.34045850919005</v>
       </c>
       <c r="C2" t="n">
-        <v>-5.023377998469892</v>
+        <v>-5.041423880421429</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-4.710269109749491</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-4.344855546796872</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +475,13 @@
         <v>-1.131202972523497</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.151483576865103</v>
+        <v>-1.155700669620174</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1.158930277919864</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.140201035762955</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +492,13 @@
         <v>-0.1981644286802984</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.06510371792358649</v>
+        <v>-0.07506705564893197</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01963012362906111</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.09302013488457662</v>
       </c>
     </row>
     <row r="5">
@@ -485,7 +509,13 @@
         <v>-0.7595660621586662</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4130396773035255</v>
+        <v>-0.4238602485323116</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.1608612870209168</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.04823066005975032</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +526,13 @@
         <v>0.07734033066112114</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01420778898168975</v>
+        <v>0.01520034001876744</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.04412375307091955</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.09856047570660458</v>
       </c>
     </row>
     <row r="7">
@@ -507,7 +543,13 @@
         <v>0.1439439259330764</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1031345171695419</v>
+        <v>0.1043279679824023</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.06603273543210547</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.02905822296111348</v>
       </c>
     </row>
     <row r="8">
@@ -518,7 +560,13 @@
         <v>0.2380344147737066</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1337589614876022</v>
+        <v>0.1352696695087812</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.03973136016071439</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.05081791680323088</v>
       </c>
     </row>
     <row r="9">
@@ -529,7 +577,13 @@
         <v>0.03166756318959256</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02733475124857185</v>
+        <v>0.02787891322180851</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.02431123640232687</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.02094463452186093</v>
       </c>
     </row>
     <row r="10">
@@ -540,7 +594,13 @@
         <v>0.03053534835443629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0234479315146108</v>
+        <v>0.02331057633078736</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01663020176682151</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.01184093569365686</v>
       </c>
     </row>
     <row r="11">
@@ -551,7 +611,13 @@
         <v>0.003002641750018904</v>
       </c>
       <c r="C11" t="n">
-        <v>0.006722294386397641</v>
+        <v>0.006819328375059187</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.00929739404265134</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.01118403691153653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
't+15' en 't+16' geloof ik allebei gelukt
</commit_message>
<xml_diff>
--- a/predicted_factors_matrix_10.xlsx
+++ b/predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,12 @@
       <c r="N1" s="1" t="n">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -520,6 +526,12 @@
       <c r="N2" t="n">
         <v>-1.090399736833865</v>
       </c>
+      <c r="O2" t="n">
+        <v>-0.8366367068726722</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.6126118682264818</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -564,6 +576,12 @@
       <c r="N3" t="n">
         <v>-0.5361955226144444</v>
       </c>
+      <c r="O3" t="n">
+        <v>-0.4657240759688368</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-0.4001321118272729</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -608,6 +626,12 @@
       <c r="N4" t="n">
         <v>0.08123680873721162</v>
       </c>
+      <c r="O4" t="n">
+        <v>0.03754329094432164</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.008940944522873105</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -652,6 +676,12 @@
       <c r="N5" t="n">
         <v>0.4523555773727749</v>
       </c>
+      <c r="O5" t="n">
+        <v>0.4166668696793512</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3768613040501999</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -696,6 +726,12 @@
       <c r="N6" t="n">
         <v>-0.3057174765299079</v>
       </c>
+      <c r="O6" t="n">
+        <v>-0.3006722170473243</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-0.2919641625736087</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -740,6 +776,12 @@
       <c r="N7" t="n">
         <v>-0.1551306753060498</v>
       </c>
+      <c r="O7" t="n">
+        <v>-0.1577104617054219</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-0.1574877845208207</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -784,6 +826,12 @@
       <c r="N8" t="n">
         <v>-0.4437392194267257</v>
       </c>
+      <c r="O8" t="n">
+        <v>-0.442120638476823</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.4342224082364093</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -828,6 +876,12 @@
       <c r="N9" t="n">
         <v>0.004288298662687616</v>
       </c>
+      <c r="O9" t="n">
+        <v>0.003556211750688697</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.002969031900047409</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -872,6 +926,12 @@
       <c r="N10" t="n">
         <v>0.005926719061297646</v>
       </c>
+      <c r="O10" t="n">
+        <v>0.006654235906479544</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.007351302360603446</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -915,6 +975,12 @@
       </c>
       <c r="N11" t="n">
         <v>0.01008760805329566</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.009029670688592699</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.007944550950589291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>